<commit_message>
Manual changes in file visin-global-defunciones-semana.csv
</commit_message>
<xml_diff>
--- a/etl/data/input/Datos_carga_semanal_demo.xlsx
+++ b/etl/data/input/Datos_carga_semanal_demo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
   <si>
     <t xml:space="preserve">Semana</t>
   </si>
@@ -209,66 +209,6 @@
   </si>
   <si>
     <t xml:space="preserve">Variación anual del acumulado en lo que va de año. De 85 y más años_España</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T</t>
   </si>
   <si>
     <t xml:space="preserve">2019SM01</t>
@@ -729,11 +669,13 @@
   </sheetPr>
   <dimension ref="A1:CE74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AH1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CF1" activeCellId="0" sqref="CF1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1965" topLeftCell="A52" activePane="topLeft" state="split"/>
+      <selection pane="topLeft" activeCell="BL1" activeCellId="0" sqref="BL1:CE1"/>
+      <selection pane="bottomLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.42"/>
@@ -939,70 +881,10 @@
       <c r="BK1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="7" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="BM1" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="BN1" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="BO1" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="BP1" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="BQ1" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="BR1" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="BS1" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="BT1" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="BU1" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="BV1" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="BW1" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="BX1" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="BY1" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="BZ1" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="CA1" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="CB1" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="CC1" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="CD1" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="CE1" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>83</v>
       </c>
       <c r="B2" s="8" t="n">
         <v>137</v>
@@ -1071,9 +953,9 @@
         <v>-952</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="B3" s="8" t="n">
         <v>164</v>
@@ -1142,9 +1024,9 @@
         <v>-1286</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B4" s="8" t="n">
         <v>160</v>
@@ -1213,9 +1095,9 @@
         <v>-1352</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="B5" s="8" t="n">
         <v>162</v>
@@ -1284,9 +1166,9 @@
         <v>-1338</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="B6" s="8" t="n">
         <v>151</v>
@@ -1355,9 +1237,9 @@
         <v>-1204</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="B7" s="8" t="n">
         <v>135</v>
@@ -1426,9 +1308,9 @@
         <v>-1474</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="B8" s="8" t="n">
         <v>133</v>
@@ -1497,9 +1379,9 @@
         <v>-1853</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="B9" s="8" t="n">
         <v>127</v>
@@ -1568,9 +1450,9 @@
         <v>-1980</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B10" s="8" t="n">
         <v>112</v>
@@ -1639,9 +1521,9 @@
         <v>-2369</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B11" s="8" t="n">
         <v>102</v>
@@ -1710,9 +1592,9 @@
         <v>-2769</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="B12" s="8" t="n">
         <v>133</v>
@@ -1781,9 +1663,9 @@
         <v>-3081</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="B13" s="8" t="n">
         <v>96</v>
@@ -1852,9 +1734,9 @@
         <v>-3482</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="B14" s="8" t="n">
         <v>116</v>
@@ -1923,9 +1805,9 @@
         <v>-3762</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="B15" s="8" t="n">
         <v>104</v>
@@ -1994,9 +1876,9 @@
         <v>-4057</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="B16" s="8" t="n">
         <v>121</v>
@@ -2065,9 +1947,9 @@
         <v>-4407</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="B17" s="8" t="n">
         <v>122</v>
@@ -2136,9 +2018,9 @@
         <v>-4583</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="B18" s="8" t="n">
         <v>110</v>
@@ -2207,9 +2089,9 @@
         <v>-4777</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="B19" s="8" t="n">
         <v>110</v>
@@ -2278,9 +2160,9 @@
         <v>-4643</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="B20" s="8" t="n">
         <v>117</v>
@@ -2349,9 +2231,9 @@
         <v>-4712</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>106</v>
@@ -2420,9 +2302,9 @@
         <v>-4765</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>119</v>
@@ -2491,9 +2373,9 @@
         <v>-4912</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>118</v>
@@ -2562,9 +2444,9 @@
         <v>-5017</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>104</v>
@@ -2633,9 +2515,9 @@
         <v>-4985</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>104</v>
@@ -2704,9 +2586,9 @@
         <v>-5098</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>102</v>
@@ -2775,9 +2657,9 @@
         <v>-5435</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>114</v>
@@ -2846,9 +2728,9 @@
         <v>-5617</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="B28" s="1" t="n">
         <v>133</v>
@@ -2917,9 +2799,9 @@
         <v>-5323</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>107</v>
@@ -2988,9 +2870,9 @@
         <v>-5352</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>100</v>
@@ -3059,9 +2941,9 @@
         <v>-5448</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>116</v>
@@ -3130,9 +3012,9 @@
         <v>-5370</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>82</v>
@@ -3201,9 +3083,9 @@
         <v>-5630</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>127</v>
@@ -3272,9 +3154,9 @@
         <v>-6003</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="B34" s="1" t="n">
         <v>107</v>
@@ -3343,9 +3225,9 @@
         <v>-6060</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="B35" s="1" t="n">
         <v>94</v>
@@ -3414,9 +3296,9 @@
         <v>-6338</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="B36" s="1" t="n">
         <v>101</v>
@@ -3485,9 +3367,9 @@
         <v>-6518</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="B37" s="1" t="n">
         <v>111</v>
@@ -3556,9 +3438,9 @@
         <v>-6807</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="B38" s="1" t="n">
         <v>103</v>
@@ -3627,9 +3509,9 @@
         <v>-7026</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="B39" s="1" t="n">
         <v>82</v>
@@ -3698,9 +3580,9 @@
         <v>-7250</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="B40" s="1" t="n">
         <v>114</v>
@@ -3769,9 +3651,9 @@
         <v>-7608</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="B41" s="1" t="n">
         <v>101</v>
@@ -3840,9 +3722,9 @@
         <v>-7832</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="B42" s="1" t="n">
         <v>92</v>
@@ -3911,9 +3793,9 @@
         <v>-8004</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="B43" s="1" t="n">
         <v>115</v>
@@ -3982,9 +3864,9 @@
         <v>-8311</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="B44" s="1" t="n">
         <v>98</v>
@@ -4053,9 +3935,9 @@
         <v>-8301</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="B45" s="1" t="n">
         <v>111</v>
@@ -4124,9 +4006,9 @@
         <v>-8487</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="B46" s="1" t="n">
         <v>115</v>
@@ -4195,9 +4077,9 @@
         <v>-8895</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="B47" s="1" t="n">
         <v>123</v>
@@ -4266,9 +4148,9 @@
         <v>-9014</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="B48" s="1" t="n">
         <v>119</v>
@@ -4337,9 +4219,9 @@
         <v>-8989</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="B49" s="1" t="n">
         <v>126</v>
@@ -4408,9 +4290,9 @@
         <v>-8974</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="B50" s="1" t="n">
         <v>102</v>
@@ -4479,9 +4361,9 @@
         <v>-9192</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="B51" s="1" t="n">
         <v>118</v>
@@ -4550,9 +4432,9 @@
         <v>-9399</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="B52" s="1" t="n">
         <v>121</v>
@@ -4621,9 +4503,9 @@
         <v>-9500</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="B53" s="1" t="n">
         <v>102</v>
@@ -4692,9 +4574,9 @@
         <v>-9858</v>
       </c>
     </row>
-    <row r="54" s="12" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="12" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="B54" s="12" t="n">
         <v>134</v>
@@ -4943,9 +4825,9 @@
         <v>0.0232018561485026</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="B55" s="1" t="n">
         <v>158</v>
@@ -5194,9 +5076,9 @@
         <v>-2.20403709765412</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="B56" s="1" t="n">
         <v>142</v>
@@ -5445,9 +5327,9 @@
         <v>-3.82981686512082</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="B57" s="1" t="n">
         <v>141</v>
@@ -5696,9 +5578,9 @@
         <v>-4.58611240370198</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="B58" s="1" t="n">
         <v>122</v>
@@ -5947,9 +5829,9 @@
         <v>-4.84953274875468</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="B59" s="1" t="n">
         <v>134</v>
@@ -6198,9 +6080,9 @@
         <v>-4.87114913581951</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="B60" s="1" t="n">
         <v>114</v>
@@ -6449,9 +6331,9 @@
         <v>-4.9859676359945</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="B61" s="1" t="n">
         <v>128</v>
@@ -6700,9 +6582,9 @@
         <v>-5.82153943284053</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B62" s="1" t="n">
         <v>119</v>
@@ -6951,9 +6833,9 @@
         <v>-6.22120360087895</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="B63" s="1" t="n">
         <v>120</v>
@@ -7202,9 +7084,9 @@
         <v>-5.75472917654156</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="B64" s="1" t="n">
         <v>112</v>
@@ -7453,9 +7335,9 @@
         <v>-4.38955567919879</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="B65" s="1" t="n">
         <v>117</v>
@@ -7704,9 +7586,9 @@
         <v>-0.116433799068527</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="B66" s="1" t="n">
         <v>137</v>
@@ -7955,9 +7837,9 @@
         <v>8.57256159588959</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="B67" s="1" t="n">
         <v>196</v>
@@ -8206,9 +8088,9 @@
         <v>18.8734490512319</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="B68" s="1" t="n">
         <v>181</v>
@@ -8457,9 +8339,9 @@
         <v>26.1828112841951</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="B69" s="1" t="n">
         <v>167</v>
@@ -8708,9 +8590,9 @@
         <v>29.5119871674446</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="B70" s="1" t="n">
         <v>152</v>
@@ -8959,9 +8841,9 @@
         <v>30.147754866856</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="B71" s="1" t="n">
         <v>127</v>
@@ -9210,9 +9092,9 @@
         <v>29.5206132389621</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
       <c r="B72" s="1" t="n">
         <v>103</v>
@@ -9461,9 +9343,9 @@
         <v>28.7502805696187</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="B73" s="1" t="n">
         <v>109</v>
@@ -9712,9 +9594,9 @@
         <v>27.3387221950258</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="B74" s="1" t="n">
         <v>87</v>

</xml_diff>

<commit_message>
Add deaths per week datasets for graphs
</commit_message>
<xml_diff>
--- a/etl/data/input/Datos_carga_semanal_demo.xlsx
+++ b/etl/data/input/Datos_carga_semanal_demo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Defunciones semanas" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,10 @@
     <sheet name="Defunciones grupos edad" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Defunciones acumuladas grupos edad" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Defunciones acumuladas grupos edad variación" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Defunciones 2019-2020" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Defunciones acumuladas 2019-2020" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Defunciones variación anual acumulado 2019-2020" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Defunciones variación anual acumulado sexo 2020" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="176">
   <si>
     <t xml:space="preserve">Semana</t>
   </si>
@@ -467,6 +471,93 @@
   </si>
   <si>
     <t xml:space="preserve">De 85 y más años</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cantabria 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cantabria 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">España 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">España 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">España Hombres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">España Mujeres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cantabria Hombres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cantabria Mujeres</t>
   </si>
 </sst>
 </file>
@@ -565,7 +656,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -627,6 +718,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -719,7 +814,7 @@
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2280" topLeftCell="A43" activePane="topLeft" state="split"/>
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+      <selection pane="topLeft" activeCell="B39" activeCellId="1" sqref="E2:E22 B39"/>
       <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
     </sheetView>
   </sheetViews>
@@ -8644,6 +8739,808 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E2:E22 A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.11"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="10" t="n">
+        <v>-22.16</v>
+      </c>
+      <c r="C2" s="10" t="n">
+        <v>-18.54</v>
+      </c>
+      <c r="D2" s="14" t="n">
+        <v>-1.93</v>
+      </c>
+      <c r="E2" s="14" t="n">
+        <v>-2.68</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="10" t="n">
+        <v>-15.92</v>
+      </c>
+      <c r="C3" s="10" t="n">
+        <v>-13.4</v>
+      </c>
+      <c r="D3" s="11" t="n">
+        <v>-2.73</v>
+      </c>
+      <c r="E3" s="11" t="n">
+        <v>-3.41</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="10" t="n">
+        <v>-11.35</v>
+      </c>
+      <c r="C4" s="10" t="n">
+        <v>-10.49</v>
+      </c>
+      <c r="D4" s="11" t="n">
+        <v>-5.69</v>
+      </c>
+      <c r="E4" s="11" t="n">
+        <v>-3.47</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" s="10" t="n">
+        <v>-7.29</v>
+      </c>
+      <c r="C5" s="10" t="n">
+        <v>-8.42</v>
+      </c>
+      <c r="D5" s="11" t="n">
+        <v>-7.63</v>
+      </c>
+      <c r="E5" s="11" t="n">
+        <v>-3.9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="10" t="n">
+        <v>-5.61</v>
+      </c>
+      <c r="C6" s="10" t="n">
+        <v>-6.72</v>
+      </c>
+      <c r="D6" s="11" t="n">
+        <v>-9.93</v>
+      </c>
+      <c r="E6" s="11" t="n">
+        <v>-3.75</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" s="10" t="n">
+        <v>-5.9</v>
+      </c>
+      <c r="C7" s="10" t="n">
+        <v>-6.19</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>-8.53</v>
+      </c>
+      <c r="E7" s="11" t="n">
+        <v>-3.61</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="10" t="n">
+        <v>-5.62</v>
+      </c>
+      <c r="C8" s="10" t="n">
+        <v>-6.36</v>
+      </c>
+      <c r="D8" s="11" t="n">
+        <v>-9.26</v>
+      </c>
+      <c r="E8" s="11" t="n">
+        <v>-3.67</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B9" s="10" t="n">
+        <v>-6.18</v>
+      </c>
+      <c r="C9" s="10" t="n">
+        <v>-6.16</v>
+      </c>
+      <c r="D9" s="11" t="n">
+        <v>-8.16</v>
+      </c>
+      <c r="E9" s="11" t="n">
+        <v>-4.15</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="10" t="n">
+        <v>-7.58</v>
+      </c>
+      <c r="C10" s="10" t="n">
+        <v>-6.25</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>-6.89</v>
+      </c>
+      <c r="E10" s="11" t="n">
+        <v>-4.79</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11" s="10" t="n">
+        <v>-8.65</v>
+      </c>
+      <c r="C11" s="10" t="n">
+        <v>-6.29</v>
+      </c>
+      <c r="D11" s="11" t="n">
+        <v>-5.05</v>
+      </c>
+      <c r="E11" s="11" t="n">
+        <v>-4.3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B12" s="10" t="n">
+        <v>-7.95</v>
+      </c>
+      <c r="C12" s="10" t="n">
+        <v>-6.38</v>
+      </c>
+      <c r="D12" s="11" t="n">
+        <v>-6.02</v>
+      </c>
+      <c r="E12" s="11" t="n">
+        <v>-2.91</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" s="10" t="n">
+        <v>-8.25</v>
+      </c>
+      <c r="C13" s="10" t="n">
+        <v>-6.42</v>
+      </c>
+      <c r="D13" s="11" t="n">
+        <v>-4.39</v>
+      </c>
+      <c r="E13" s="11" t="n">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" s="10" t="n">
+        <v>-7.1</v>
+      </c>
+      <c r="C14" s="10" t="n">
+        <v>-6.35</v>
+      </c>
+      <c r="D14" s="11" t="n">
+        <v>-2.88</v>
+      </c>
+      <c r="E14" s="11" t="n">
+        <v>10.51</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="10" t="n">
+        <v>-7.61</v>
+      </c>
+      <c r="C15" s="10" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="D15" s="11" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="E15" s="11" t="n">
+        <v>19.61</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="10" t="n">
+        <v>-7.44</v>
+      </c>
+      <c r="C16" s="10" t="n">
+        <v>-6.04</v>
+      </c>
+      <c r="D16" s="11" t="n">
+        <v>5.27</v>
+      </c>
+      <c r="E16" s="11" t="n">
+        <v>25.18</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" s="10" t="n">
+        <v>-6.19</v>
+      </c>
+      <c r="C17" s="10" t="n">
+        <v>-5.92</v>
+      </c>
+      <c r="D17" s="11" t="n">
+        <v>7.14</v>
+      </c>
+      <c r="E17" s="11" t="n">
+        <v>27.49</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B18" s="10" t="n">
+        <v>-5.62</v>
+      </c>
+      <c r="C18" s="10" t="n">
+        <v>-5.63</v>
+      </c>
+      <c r="D18" s="11" t="n">
+        <v>8.71</v>
+      </c>
+      <c r="E18" s="11" t="n">
+        <v>27.76</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B19" s="10" t="n">
+        <v>-5.28</v>
+      </c>
+      <c r="C19" s="10" t="n">
+        <v>-5.15</v>
+      </c>
+      <c r="D19" s="11" t="n">
+        <v>9.02</v>
+      </c>
+      <c r="E19" s="11" t="n">
+        <v>27.07</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20" s="10" t="n">
+        <v>-4.51</v>
+      </c>
+      <c r="C20" s="10" t="n">
+        <v>-4.85</v>
+      </c>
+      <c r="D20" s="11" t="n">
+        <v>7.99</v>
+      </c>
+      <c r="E20" s="11" t="n">
+        <v>26.3</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B21" s="11" t="n">
+        <v>-4.69</v>
+      </c>
+      <c r="C21" s="11" t="n">
+        <v>-4.64</v>
+      </c>
+      <c r="D21" s="11" t="n">
+        <v>7.77</v>
+      </c>
+      <c r="E21" s="11" t="n">
+        <v>25.15</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" s="11" t="n">
+        <v>-4.11</v>
+      </c>
+      <c r="C22" s="11" t="n">
+        <v>-4.51</v>
+      </c>
+      <c r="D22" s="11" t="n">
+        <v>6.23</v>
+      </c>
+      <c r="E22" s="11" t="n">
+        <v>24.15</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="14" t="n">
+        <v>-3.06321963936563</v>
+      </c>
+      <c r="C2" s="14" t="n">
+        <v>-2.29885057471264</v>
+      </c>
+      <c r="D2" s="14" t="n">
+        <v>-7.93650793650794</v>
+      </c>
+      <c r="E2" s="14" t="n">
+        <v>2.7027027027027</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="11" t="n">
+        <v>-4.02747424289729</v>
+      </c>
+      <c r="C3" s="11" t="n">
+        <v>-2.78913704519241</v>
+      </c>
+      <c r="D3" s="11" t="n">
+        <v>-4.72972972972973</v>
+      </c>
+      <c r="E3" s="11" t="n">
+        <v>-0.653594771241828</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="11" t="n">
+        <v>-3.72750642673522</v>
+      </c>
+      <c r="C4" s="11" t="n">
+        <v>-3.20145581990968</v>
+      </c>
+      <c r="D4" s="11" t="n">
+        <v>-6.25</v>
+      </c>
+      <c r="E4" s="11" t="n">
+        <v>-5.48523206751055</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" s="11" t="n">
+        <v>-3.30428650581775</v>
+      </c>
+      <c r="C5" s="11" t="n">
+        <v>-4.4908826041091</v>
+      </c>
+      <c r="D5" s="11" t="n">
+        <v>-2.7027027027027</v>
+      </c>
+      <c r="E5" s="11" t="n">
+        <v>-11.9266055045872</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="11" t="n">
+        <v>-2.99386701097483</v>
+      </c>
+      <c r="C6" s="11" t="n">
+        <v>-4.49478748997594</v>
+      </c>
+      <c r="D6" s="11" t="n">
+        <v>-5.46448087431694</v>
+      </c>
+      <c r="E6" s="11" t="n">
+        <v>-13.9705882352941</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" s="11" t="n">
+        <v>-3.14439946018893</v>
+      </c>
+      <c r="C7" s="11" t="n">
+        <v>-4.07594086021506</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>-5.42452830188679</v>
+      </c>
+      <c r="E7" s="11" t="n">
+        <v>-11.1340206185567</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="11" t="n">
+        <v>-3.12409014150119</v>
+      </c>
+      <c r="C8" s="11" t="n">
+        <v>-4.21376885298306</v>
+      </c>
+      <c r="D8" s="11" t="n">
+        <v>-6.12244897959183</v>
+      </c>
+      <c r="E8" s="11" t="n">
+        <v>-12.1376811594203</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B9" s="11" t="n">
+        <v>-3.68239946587232</v>
+      </c>
+      <c r="C9" s="11" t="n">
+        <v>-4.6252402306214</v>
+      </c>
+      <c r="D9" s="11" t="n">
+        <v>-6.63082437275986</v>
+      </c>
+      <c r="E9" s="11" t="n">
+        <v>-9.49263502454992</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="11" t="n">
+        <v>-4.3581252012327</v>
+      </c>
+      <c r="C10" s="11" t="n">
+        <v>-5.21841304948852</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>-5.7784911717496</v>
+      </c>
+      <c r="E10" s="11" t="n">
+        <v>-7.90273556231003</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11" s="11" t="n">
+        <v>-3.76408134261291</v>
+      </c>
+      <c r="C11" s="11" t="n">
+        <v>-4.83129317403993</v>
+      </c>
+      <c r="D11" s="11" t="n">
+        <v>-3.27380952380952</v>
+      </c>
+      <c r="E11" s="11" t="n">
+        <v>-6.75105485232067</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B12" s="11" t="n">
+        <v>-2.04179909467399</v>
+      </c>
+      <c r="C12" s="11" t="n">
+        <v>-3.78277081200131</v>
+      </c>
+      <c r="D12" s="11" t="n">
+        <v>-3.5374149659864</v>
+      </c>
+      <c r="E12" s="11" t="n">
+        <v>-8.32266325224071</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" s="11" t="n">
+        <v>2.97077400706562</v>
+      </c>
+      <c r="C13" s="11" t="n">
+        <v>-0.0952346726083464</v>
+      </c>
+      <c r="D13" s="11" t="n">
+        <v>-2.78128950695322</v>
+      </c>
+      <c r="E13" s="11" t="n">
+        <v>-5.96833130328868</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" s="11" t="n">
+        <v>12.9451235716184</v>
+      </c>
+      <c r="C14" s="11" t="n">
+        <v>8.04405035283864</v>
+      </c>
+      <c r="D14" s="11" t="n">
+        <v>-0.117924528301883</v>
+      </c>
+      <c r="E14" s="11" t="n">
+        <v>-5.56818181818182</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="11" t="n">
+        <v>21.9610403743606</v>
+      </c>
+      <c r="C15" s="11" t="n">
+        <v>17.2259332023576</v>
+      </c>
+      <c r="D15" s="11" t="n">
+        <v>4.55049944506105</v>
+      </c>
+      <c r="E15" s="11" t="n">
+        <v>0.214822771213741</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="11" t="n">
+        <v>26.4416622891496</v>
+      </c>
+      <c r="C16" s="11" t="n">
+        <v>23.890906395909</v>
+      </c>
+      <c r="D16" s="11" t="n">
+        <v>7.56476683937823</v>
+      </c>
+      <c r="E16" s="11" t="n">
+        <v>3.03643724696356</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" s="11" t="n">
+        <v>28.1305662565759</v>
+      </c>
+      <c r="C17" s="11" t="n">
+        <v>26.8437570051558</v>
+      </c>
+      <c r="D17" s="11" t="n">
+        <v>9.49119373776908</v>
+      </c>
+      <c r="E17" s="11" t="n">
+        <v>4.84330484330484</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B18" s="11" t="n">
+        <v>27.9310750873337</v>
+      </c>
+      <c r="C18" s="11" t="n">
+        <v>27.5751444317244</v>
+      </c>
+      <c r="D18" s="11" t="n">
+        <v>11.9402985074627</v>
+      </c>
+      <c r="E18" s="11" t="n">
+        <v>5.57053009883199</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B19" s="11" t="n">
+        <v>27.1371992228366</v>
+      </c>
+      <c r="C19" s="11" t="n">
+        <v>26.9989747224789</v>
+      </c>
+      <c r="D19" s="11" t="n">
+        <v>11.790780141844</v>
+      </c>
+      <c r="E19" s="11" t="n">
+        <v>6.34104541559555</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20" s="11" t="n">
+        <v>26.1370786783649</v>
+      </c>
+      <c r="C20" s="11" t="n">
+        <v>26.4723644796599</v>
+      </c>
+      <c r="D20" s="11" t="n">
+        <v>10.042194092827</v>
+      </c>
+      <c r="E20" s="11" t="n">
+        <v>5.94947025264874</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B21" s="11" t="n">
+        <v>25.035224070539</v>
+      </c>
+      <c r="C21" s="11" t="n">
+        <v>25.2703701991958</v>
+      </c>
+      <c r="D21" s="11" t="n">
+        <v>9.03954802259888</v>
+      </c>
+      <c r="E21" s="11" t="n">
+        <v>6.56763096168882</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" s="11" t="n">
+        <v>23.9804650452945</v>
+      </c>
+      <c r="C22" s="11" t="n">
+        <v>24.3174666489385</v>
+      </c>
+      <c r="D22" s="11" t="n">
+        <v>7.01078582434516</v>
+      </c>
+      <c r="E22" s="11" t="n">
+        <v>5.45182972367437</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -8652,31 +9549,34 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="E2:E22 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="16" t="s">
         <v>141</v>
       </c>
     </row>
@@ -9182,31 +10082,34 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="E2:E22 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="16" t="s">
         <v>141</v>
       </c>
     </row>
@@ -9712,31 +10615,34 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="E2:E22 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="16" t="s">
         <v>141</v>
       </c>
     </row>
@@ -10242,28 +11148,31 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="E2:E22 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="18" t="s">
         <v>146</v>
       </c>
     </row>
@@ -10706,28 +11615,31 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="E2:E22 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="18" t="s">
         <v>146</v>
       </c>
     </row>
@@ -11169,29 +12081,32 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="E2:E22 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="18" t="s">
         <v>146</v>
       </c>
     </row>
@@ -11613,6 +12528,546 @@
       </c>
       <c r="F22" s="11" t="n">
         <v>-0.362056480811002</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="E2:E22 A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.69"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="8" t="n">
+        <v>137</v>
+      </c>
+      <c r="C2" s="12" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="8" t="n">
+        <v>164</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="8" t="n">
+        <v>160</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" s="8" t="n">
+        <v>162</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="8" t="n">
+        <v>151</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" s="8" t="n">
+        <v>135</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="8" t="n">
+        <v>133</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B9" s="8" t="n">
+        <v>127</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="8" t="n">
+        <v>112</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11" s="8" t="n">
+        <v>102</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B12" s="8" t="n">
+        <v>133</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" s="8" t="n">
+        <v>96</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" s="8" t="n">
+        <v>116</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="8" t="n">
+        <v>104</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="8" t="n">
+        <v>121</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" s="8" t="n">
+        <v>122</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B18" s="8" t="n">
+        <v>110</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B19" s="8" t="n">
+        <v>110</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20" s="8" t="n">
+        <v>117</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E2:E22 A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.44"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="9" t="n">
+        <v>137</v>
+      </c>
+      <c r="C2" s="13" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="9" t="n">
+        <v>301</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="9" t="n">
+        <v>461</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" s="9" t="n">
+        <v>623</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="9" t="n">
+        <v>774</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" s="9" t="n">
+        <v>909</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="9" t="n">
+        <v>1042</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B9" s="9" t="n">
+        <v>1169</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="9" t="n">
+        <v>1281</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11" s="9" t="n">
+        <v>1383</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B12" s="9" t="n">
+        <v>1516</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" s="9" t="n">
+        <v>1612</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" s="9" t="n">
+        <v>1728</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="9" t="n">
+        <v>1832</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="9" t="n">
+        <v>1953</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2056</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" s="9" t="n">
+        <v>2075</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>2223</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B18" s="9" t="n">
+        <v>2185</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>2375</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B19" s="9" t="n">
+        <v>2295</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>2502</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20" s="9" t="n">
+        <v>2412</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>2605</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>2518</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>2714</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>2637</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>2801</v>
       </c>
     </row>
   </sheetData>

</xml_diff>